<commit_message>
end adding vlm to simu
</commit_message>
<xml_diff>
--- a/OZONE/polar_c_alphafind_cg.xlsx
+++ b/OZONE/polar_c_alphafind_cg.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AN6"/>
+  <dimension ref="A1:AN2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -772,574 +772,6 @@
         <v>5.016084264779372</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>8</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.1533</v>
-      </c>
-      <c r="E3" t="n">
-        <v>1.3797</v>
-      </c>
-      <c r="F3" t="n">
-        <v>-0.1896449495794474</v>
-      </c>
-      <c r="G3" t="n">
-        <v>3.517932727244638</v>
-      </c>
-      <c r="H3" t="n">
-        <v>1.562119930831016</v>
-      </c>
-      <c r="I3" t="n">
-        <v>75.39512562201935</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.7859965811719768</v>
-      </c>
-      <c r="K3" t="n">
-        <v>-1.13686837721616e-12</v>
-      </c>
-      <c r="L3" t="n">
-        <v>31.81200303160785</v>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>[0.7005900950306444, 0, -0.043070024644796076]</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>[0.06657060551902136, 0, -0.004092546612720573]</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>[31.809009731523833, 0, 0.4363906310278392]</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>[17.25640311624275, 0, 0.23674212774077422]</t>
-        </is>
-      </c>
-      <c r="Q3" t="n">
-        <v>794.908427904442</v>
-      </c>
-      <c r="R3" t="n">
-        <v>215.6622940542995</v>
-      </c>
-      <c r="S3" t="n">
-        <v>15</v>
-      </c>
-      <c r="T3" t="n">
-        <v>1500.056461656201</v>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>[1.30149205e+01 6.58958998e-13 1.50000000e+03]</t>
-        </is>
-      </c>
-      <c r="V3" t="inlineStr">
-        <is>
-          <t>(np.float64(-13.014920534534792), np.float64(6.589589984784539e-13), np.float64(-1500.0))</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>(np.float64(-33.59039289094954), np.float64(6.589589984784539e-13), np.float64(-1499.6803238230311))</t>
-        </is>
-      </c>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t>[ 2.49333887e-12 -1.05286912e+03  2.63816746e-13]</t>
-        </is>
-      </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t>(np.float64(-2.4933388687031766e-12), np.float64(-1052.8691246424637), np.float64(-2.638167462265528e-13))</t>
-        </is>
-      </c>
-      <c r="Z3" t="inlineStr">
-        <is>
-          <t>(np.float64(-2.496723246757252e-12), np.float64(-1052.8691246424637), np.float64(-2.295888039028208e-13))</t>
-        </is>
-      </c>
-      <c r="AA3" t="n">
-        <v>1499.680323823031</v>
-      </c>
-      <c r="AB3" t="n">
-        <v>33.59039289094954</v>
-      </c>
-      <c r="AC3" t="n">
-        <v>6.589589984784539e-13</v>
-      </c>
-      <c r="AD3" t="n">
-        <v>-2.493338868703177e-12</v>
-      </c>
-      <c r="AE3" t="n">
-        <v>-1052.869124642464</v>
-      </c>
-      <c r="AF3" t="n">
-        <v>-2.638167462265528e-13</v>
-      </c>
-      <c r="AG3" t="n">
-        <v>0.4076064504462784</v>
-      </c>
-      <c r="AH3" t="n">
-        <v>0.009129719579485208</v>
-      </c>
-      <c r="AI3" t="n">
-        <v>1.791021286954836e-16</v>
-      </c>
-      <c r="AJ3" t="n">
-        <v>-4.075167205456397e-17</v>
-      </c>
-      <c r="AK3" t="n">
-        <v>-0.1620445657928292</v>
-      </c>
-      <c r="AL3" t="n">
-        <v>-4.311878204633432e-18</v>
-      </c>
-      <c r="AM3" t="n">
-        <v>44.64610844808246</v>
-      </c>
-      <c r="AN3" t="n">
-        <v>4.303929308416615</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>8</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.1533</v>
-      </c>
-      <c r="E4" t="n">
-        <v>1.3797</v>
-      </c>
-      <c r="F4" t="n">
-        <v>-0.1909970824950261</v>
-      </c>
-      <c r="G4" t="n">
-        <v>2.946489287743263</v>
-      </c>
-      <c r="H4" t="n">
-        <v>1.565399667157822</v>
-      </c>
-      <c r="I4" t="n">
-        <v>63.12442881137199</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.7890957343093216</v>
-      </c>
-      <c r="K4" t="n">
-        <v>1.15164766611997e-10</v>
-      </c>
-      <c r="L4" t="n">
-        <v>35.21645237761999</v>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>[0.6939620474115085, 0, -0.035719143721152743]</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>[0.06810784147814511, 0, -0.0035056006122662913]</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>[35.21311255908742, 0, 0.4849968723775836]</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>[19.63393739152041, 0, 0.27042194044522916]</t>
-        </is>
-      </c>
-      <c r="Q4" t="n">
-        <v>879.9952182456291</v>
-      </c>
-      <c r="R4" t="n">
-        <v>245.3751172256683</v>
-      </c>
-      <c r="S4" t="n">
-        <v>16</v>
-      </c>
-      <c r="T4" t="n">
-        <v>1500.021843216493</v>
-      </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>[ 8.09506804e+00 -1.71085368e-13  1.50000000e+03]</t>
-        </is>
-      </c>
-      <c r="V4" t="inlineStr">
-        <is>
-          <t>(np.float64(-8.09506804250981), np.float64(-1.7108536809473662e-13), np.float64(-1499.999999999998))</t>
-        </is>
-      </c>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t>(np.float64(-28.75212528120001), np.float64(-1.7108536809473662e-13), np.float64(-1499.7462603448696))</t>
-        </is>
-      </c>
-      <c r="X4" t="inlineStr">
-        <is>
-          <t>[ 9.97091298e-13 -1.04232104e+03 -3.80445675e-13]</t>
-        </is>
-      </c>
-      <c r="Y4" t="inlineStr">
-        <is>
-          <t>(np.float64(-9.97091298415853e-13), np.float64(-1042.321042707297), np.float64(3.804456749634255e-13))</t>
-        </is>
-      </c>
-      <c r="Z4" t="inlineStr">
-        <is>
-          <t>(np.float64(-9.917572839487024e-13), np.float64(-1042.321042707297), np.float64(3.94141419682937e-13))</t>
-        </is>
-      </c>
-      <c r="AA4" t="n">
-        <v>1499.74626034487</v>
-      </c>
-      <c r="AB4" t="n">
-        <v>28.75212528120001</v>
-      </c>
-      <c r="AC4" t="n">
-        <v>-1.710853680947366e-13</v>
-      </c>
-      <c r="AD4" t="n">
-        <v>-9.970912984158531e-13</v>
-      </c>
-      <c r="AE4" t="n">
-        <v>-1042.321042707297</v>
-      </c>
-      <c r="AF4" t="n">
-        <v>3.804456749634255e-13</v>
-      </c>
-      <c r="AG4" t="n">
-        <v>0.3582636079394747</v>
-      </c>
-      <c r="AH4" t="n">
-        <v>0.006868388614485892</v>
-      </c>
-      <c r="AI4" t="n">
-        <v>-4.086935427675535e-17</v>
-      </c>
-      <c r="AJ4" t="n">
-        <v>-1.432325106039238e-17</v>
-      </c>
-      <c r="AK4" t="n">
-        <v>-0.1409951388519397</v>
-      </c>
-      <c r="AL4" t="n">
-        <v>5.465115306892283e-18</v>
-      </c>
-      <c r="AM4" t="n">
-        <v>52.16123141079593</v>
-      </c>
-      <c r="AN4" t="n">
-        <v>3.735585022052585</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>8</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.1533</v>
-      </c>
-      <c r="E5" t="n">
-        <v>1.3797</v>
-      </c>
-      <c r="F5" t="n">
-        <v>-0.2009772943239635</v>
-      </c>
-      <c r="G5" t="n">
-        <v>2.464392587877553</v>
-      </c>
-      <c r="H5" t="n">
-        <v>1.568461029240809</v>
-      </c>
-      <c r="I5" t="n">
-        <v>52.78218148936334</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0.8119709278751488</v>
-      </c>
-      <c r="K5" t="n">
-        <v>1.926991899381392e-10</v>
-      </c>
-      <c r="L5" t="n">
-        <v>38.79185151031787</v>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>[0.688219799374881, 0, -0.029619816010419266]</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>[0.07060452651562721, 0, -0.0030386993905075024]</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>[38.78795622799923, 0, 0.5497228877956948]</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>[22.164750984208567, 0, 0.31413026370067404]</t>
-        </is>
-      </c>
-      <c r="Q5" t="n">
-        <v>969.3343737388567</v>
-      </c>
-      <c r="R5" t="n">
-        <v>276.9999998693609</v>
-      </c>
-      <c r="S5" t="n">
-        <v>17</v>
-      </c>
-      <c r="T5" t="n">
-        <v>1500.004090220288</v>
-      </c>
-      <c r="U5" t="inlineStr">
-        <is>
-          <t>[3.5029527e+00 2.1034563e-13 1.5000000e+03]</t>
-        </is>
-      </c>
-      <c r="V5" t="inlineStr">
-        <is>
-          <t>(np.float64(-3.502952699051309), np.float64(2.1034562980304372e-13), np.float64(-1499.9999999999939))</t>
-        </is>
-      </c>
-      <c r="W5" t="inlineStr">
-        <is>
-          <t>(np.float64(-24.75923860962476), np.float64(2.1034562980304372e-13), np.float64(-1499.7997368919175))</t>
-        </is>
-      </c>
-      <c r="X5" t="inlineStr">
-        <is>
-          <t>[-1.46449519e-12 -1.03328535e+03  2.09651740e-13]</t>
-        </is>
-      </c>
-      <c r="Y5" t="inlineStr">
-        <is>
-          <t>(np.float64(1.464495191783044e-12), np.float64(-1033.2853468148096), np.float64(-2.09651740412653e-13))</t>
-        </is>
-      </c>
-      <c r="Z5" t="inlineStr">
-        <is>
-          <t>(np.float64(1.4613771404993833e-12), np.float64(-1033.2853468148096), np.float64(-2.3038418400479423e-13))</t>
-        </is>
-      </c>
-      <c r="AA5" t="n">
-        <v>1499.799736891918</v>
-      </c>
-      <c r="AB5" t="n">
-        <v>24.75923860962476</v>
-      </c>
-      <c r="AC5" t="n">
-        <v>2.103456298030437e-13</v>
-      </c>
-      <c r="AD5" t="n">
-        <v>1.464495191783044e-12</v>
-      </c>
-      <c r="AE5" t="n">
-        <v>-1033.28534681481</v>
-      </c>
-      <c r="AF5" t="n">
-        <v>-2.09651740412653e-13</v>
-      </c>
-      <c r="AG5" t="n">
-        <v>0.3173659305788692</v>
-      </c>
-      <c r="AH5" t="n">
-        <v>0.005239192012429387</v>
-      </c>
-      <c r="AI5" t="n">
-        <v>4.451030021113551e-17</v>
-      </c>
-      <c r="AJ5" t="n">
-        <v>1.863531554420917e-17</v>
-      </c>
-      <c r="AK5" t="n">
-        <v>-0.1238126523339911</v>
-      </c>
-      <c r="AL5" t="n">
-        <v>-2.667763171161852e-18</v>
-      </c>
-      <c r="AM5" t="n">
-        <v>60.57535777004443</v>
-      </c>
-      <c r="AN5" t="n">
-        <v>3.276363515752702</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>8</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.1533</v>
-      </c>
-      <c r="E6" t="n">
-        <v>1.3797</v>
-      </c>
-      <c r="F6" t="n">
-        <v>-0.2183821518771462</v>
-      </c>
-      <c r="G6" t="n">
-        <v>2.050040871818755</v>
-      </c>
-      <c r="H6" t="n">
-        <v>1.570219210690919</v>
-      </c>
-      <c r="I6" t="n">
-        <v>43.89928160998554</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0.8518641290159507</v>
-      </c>
-      <c r="K6" t="n">
-        <v>5.002220859751105e-12</v>
-      </c>
-      <c r="L6" t="n">
-        <v>42.55773428397666</v>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>[0.683170040210646, 0, -0.024454235145721048]</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>[0.07370810227209128, 0, -0.002638399167139718]</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>[42.55303062421048, 0, 0.6327180103073698]</t>
-        </is>
-      </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>[24.848812156697523, 0, 0.3694752349164543]</t>
-        </is>
-      </c>
-      <c r="Q6" t="n">
-        <v>1063.41110446282</v>
-      </c>
-      <c r="R6" t="n">
-        <v>310.5354786200455</v>
-      </c>
-      <c r="S6" t="n">
-        <v>18</v>
-      </c>
-      <c r="T6" t="n">
-        <v>1500.000249797284</v>
-      </c>
-      <c r="U6" t="inlineStr">
-        <is>
-          <t>[-8.65674252e-01  3.80390164e-14  1.50000000e+03]</t>
-        </is>
-      </c>
-      <c r="V6" t="inlineStr">
-        <is>
-          <t>(np.float64(0.8656742520744805), np.float64(3.8039016381219426e-14), np.float64(-1500.000000000001))</t>
-        </is>
-      </c>
-      <c r="W6" t="inlineStr">
-        <is>
-          <t>(np.float64(-21.43535053851317), np.float64(3.8039016381219426e-14), np.float64(-1499.8470839186255))</t>
-        </is>
-      </c>
-      <c r="X6" t="inlineStr">
-        <is>
-          <t>[-3.64708264e-13 -1.02541136e+03  1.05263021e-13]</t>
-        </is>
-      </c>
-      <c r="Y6" t="inlineStr">
-        <is>
-          <t>(np.float64(3.647082635893639e-13), np.float64(-1025.4113590556979), np.float64(-1.0526302052227265e-13))</t>
-        </is>
-      </c>
-      <c r="Z6" t="inlineStr">
-        <is>
-          <t>(np.float64(3.6310297905908865e-13), np.float64(-1025.4113590556979), np.float64(-1.106736084993003e-13))</t>
-        </is>
-      </c>
-      <c r="AA6" t="n">
-        <v>1499.847083918625</v>
-      </c>
-      <c r="AB6" t="n">
-        <v>21.43535053851317</v>
-      </c>
-      <c r="AC6" t="n">
-        <v>3.803901638121943e-14</v>
-      </c>
-      <c r="AD6" t="n">
-        <v>3.647082635893639e-13</v>
-      </c>
-      <c r="AE6" t="n">
-        <v>-1025.411359055698</v>
-      </c>
-      <c r="AF6" t="n">
-        <v>-1.052630205222727e-13</v>
-      </c>
-      <c r="AG6" t="n">
-        <v>0.2830915104857735</v>
-      </c>
-      <c r="AH6" t="n">
-        <v>0.004045856292153155</v>
-      </c>
-      <c r="AI6" t="n">
-        <v>7.1797470023529e-18</v>
-      </c>
-      <c r="AJ6" t="n">
-        <v>4.139493805079439e-18</v>
-      </c>
-      <c r="AK6" t="n">
-        <v>-0.1095962547508518</v>
-      </c>
-      <c r="AL6" t="n">
-        <v>-1.19475116101703e-18</v>
-      </c>
-      <c r="AM6" t="n">
-        <v>69.9707280841445</v>
-      </c>
-      <c r="AN6" t="n">
-        <v>2.901905000834706</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>